<commit_message>
Spring Security Method Security Hello World
</commit_message>
<xml_diff>
--- a/java/spring-security/doc/image.xlsx
+++ b/java/spring-security/doc/image.xlsx
@@ -87,8 +87,8 @@
     <xdr:to>
       <xdr:col>53</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>98758</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>32556</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -97,8 +97,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1576753" y="3033347"/>
-          <a:ext cx="3859824" cy="3806180"/>
+          <a:off x="1609724" y="3086101"/>
+          <a:ext cx="3943351" cy="3633005"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -152,8 +152,8 @@
     <xdr:to>
       <xdr:col>52</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>167786</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>102024</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -162,8 +162,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1474176" y="2941027"/>
-          <a:ext cx="3859824" cy="3799009"/>
+          <a:off x="1504949" y="2990850"/>
+          <a:ext cx="3943351" cy="3626274"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -217,8 +217,8 @@
     <xdr:to>
       <xdr:col>51</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>65942</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -227,8 +227,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1371599" y="2839183"/>
-          <a:ext cx="3859824" cy="3799009"/>
+          <a:off x="1400174" y="2886075"/>
+          <a:ext cx="3943351" cy="3629025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -476,14 +476,14 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>47628</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47627</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>48</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -492,8 +492,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1586282" y="5684961"/>
-          <a:ext cx="3337410" cy="524607"/>
+          <a:off x="1619253" y="5876927"/>
+          <a:ext cx="3409947" cy="342898"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -542,16 +542,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>63</xdr:col>
-      <xdr:colOff>91940</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>29988</xdr:rowOff>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>15740</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>39513</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>90</xdr:col>
-      <xdr:colOff>67284</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>49035</xdr:rowOff>
+      <xdr:colOff>95859</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>58560</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -560,8 +560,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6554286" y="5254084"/>
-          <a:ext cx="2744921" cy="524605"/>
+          <a:off x="6721340" y="3982863"/>
+          <a:ext cx="2804269" cy="533397"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -608,15 +608,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>131</xdr:colOff>
+      <xdr:colOff>19181</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>144816</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>90</xdr:col>
+      <xdr:colOff>93180</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>59091</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>90</xdr:col>
-      <xdr:colOff>74130</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>78139</xdr:rowOff>
+      <xdr:rowOff>163864</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -625,8 +625,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6565054" y="6125783"/>
-          <a:ext cx="2740999" cy="524606"/>
+          <a:off x="6724781" y="5802666"/>
+          <a:ext cx="2798149" cy="533398"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -672,16 +672,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>57148</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>67406</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>49</xdr:col>
-      <xdr:colOff>85726</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>150201</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38098</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>124556</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>35901</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -690,8 +690,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1185494" y="7313733"/>
-          <a:ext cx="3926501" cy="925391"/>
+          <a:off x="1295398" y="7154006"/>
+          <a:ext cx="4010028" cy="940045"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -783,7 +783,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -791,9 +791,9 @@
               <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>CsrfFilter</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400">
+            <a:t>UsernamePasswordAuthenticationFilter</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
             </a:solidFill>
@@ -1314,26 +1314,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>49</xdr:col>
-      <xdr:colOff>62010</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>66641</xdr:rowOff>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>92949</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>63</xdr:col>
-      <xdr:colOff>9466</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>119750</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="下矢印 21"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="15545327">
-          <a:off x="5584972" y="4962563"/>
-          <a:ext cx="390148" cy="1383533"/>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>64917</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="下矢印 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="5548041" y="5279583"/>
+          <a:ext cx="703092" cy="1554876"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst>
@@ -1369,26 +1369,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>22712</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>84992</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>62</xdr:col>
-      <xdr:colOff>58613</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>46892</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="正方形/長方形 23"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5254135" y="5140569"/>
-          <a:ext cx="1164247" cy="298938"/>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>88342</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>85411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>20828</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>52963</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="正方形/長方形 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5222317" y="5914711"/>
+          <a:ext cx="1189786" cy="310452"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1430,35 +1430,35 @@
               <a:latin typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
               <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
             </a:rPr>
-            <a:t>認証処理</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>49</xdr:col>
-      <xdr:colOff>54849</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>461</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>62</xdr:col>
-      <xdr:colOff>92144</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>54931</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="下矢印 24"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16761539">
-          <a:off x="5570761" y="5577510"/>
-          <a:ext cx="391509" cy="1370795"/>
+            <a:t>認可処理</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="下矢印 26"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3019425" y="6343651"/>
+          <a:ext cx="542925" cy="723900"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst>
@@ -1494,26 +1494,136 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>31192</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>142561</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>62</xdr:col>
-      <xdr:colOff>68453</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>110113</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="正方形/長方形 25"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5262615" y="6546292"/>
-          <a:ext cx="1165607" cy="304590"/>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="下矢印 27"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3019425" y="123825"/>
+          <a:ext cx="542925" cy="485776"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj2" fmla="val 46970"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>92949</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>141117</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="下矢印 28"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="5548041" y="3469833"/>
+          <a:ext cx="703092" cy="1554876"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj2" fmla="val 46970"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>3662</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>151667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>39563</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>113567</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="正方形/長方形 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5242412" y="4095017"/>
+          <a:ext cx="1188426" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1555,118 +1665,8 @@
               <a:latin typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
               <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
             </a:rPr>
-            <a:t>認可処理</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>153865</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="下矢印 26"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2957879" y="6387612"/>
-          <a:ext cx="529736" cy="844061"/>
-        </a:xfrm>
-        <a:prstGeom prst="downArrow">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-            <a:gd name="adj2" fmla="val 46970"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="下矢印 27"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3019425" y="123825"/>
-          <a:ext cx="542925" cy="485776"/>
-        </a:xfrm>
-        <a:prstGeom prst="downArrow">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-            <a:gd name="adj2" fmla="val 46970"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>認証処理</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1965,7 +1965,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CT43" sqref="CT43"/>
+      <selection activeCell="EX21" sqref="EX21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.375" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>